<commit_message>
Finish Story folder structure, Finish Ogier story file
</commit_message>
<xml_diff>
--- a/Story/3 - Psyche Deepdive/1 - The Knight's Wish/The Knight's Wish.xlsx
+++ b/Story/3 - Psyche Deepdive/1 - The Knight's Wish/The Knight's Wish.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theda\Documents\GitHub\morimens-volunteer-coordination\Story\3 - Psyche Deepdive\1 - The Knight's Wish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46DD42B-095C-4F2D-A1F8-9B763047A3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C018674C-C6C7-434E-9A89-D8D43864AD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="20850" windowHeight="16305" xr2:uid="{AF0DFFA9-3CB3-46E1-8EB3-1DEAB25BEACF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AF0DFFA9-3CB3-46E1-8EB3-1DEAB25BEACF}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ogier Story" sheetId="1" r:id="rId1"/>
+    <sheet name="Ogier Deepdive" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -15595,9 +15595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21EBE32-BDBF-4AFC-BED4-949DC701710C}">
   <dimension ref="A1:S414"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A395" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Finish compiling base repo contributions
</commit_message>
<xml_diff>
--- a/Story/3 - Psyche Deepdive/1 - The Knight's Wish/The Knight's Wish.xlsx
+++ b/Story/3 - Psyche Deepdive/1 - The Knight's Wish/The Knight's Wish.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theda\Documents\GitHub\morimens-volunteer-coordination\Story\3 - Psyche Deepdive\1 - The Knight's Wish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C018674C-C6C7-434E-9A89-D8D43864AD5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3023F5-0869-4516-B1A7-C1E761277879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{AF0DFFA9-3CB3-46E1-8EB3-1DEAB25BEACF}"/>
   </bookViews>
@@ -14993,9 +14993,6 @@
     <t>霊と心の共鳴により、あなたは彼らの記憶に入り、彼らの夢を見ることができます。\n愛と苦しみを実際に体験し、壮絶な瞬間と温かい情景を目撃してください。これによって、あなたは感情の壮大さを理解することができるでしょう。</t>
   </si>
   <si>
-    <t>영혼과 마음의 공명은 당신이 그들의 기억, 그들의 꿈에 들어갈 수 있게 합니다. \n 사랑과 고통을 직접 경험하고, 장엄함과 따뜻함을 목격하세요. 이렇게 하여야만 감정의 거대함을 이해할 수 있습니다.</t>
-  </si>
-  <si>
     <t>La résonance de l'âme et du cœur te permet d'entrer dans leurs souvenirs, dans leurs rêves.\nVis l'amour et la douleur, sois témoin de la grandeur et de la tendresse. Ainsi, tu comprendras l'ampleur des émotions</t>
   </si>
   <si>
@@ -15324,13 +15321,16 @@
   </si>
   <si>
     <t>Stage_20435_Name</t>
+  </si>
+  <si>
+    <t>당신은 영혼과 마음의 공명을 통해 그들의 기억과 꿈 속에 들어갈 수 있게 되었다.\n사랑과 고통을 경험하고, 영광과 온정을 목도하라. 그래야만 비로소 감정의 웅대한 힘을 이해할 수 있을 것이다.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -15341,6 +15341,17 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -15367,10 +15378,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -15378,9 +15390,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{DB082697-9283-40C9-95E6-CA3885F56CB3}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -15595,7 +15611,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21EBE32-BDBF-4AFC-BED4-949DC701710C}">
   <dimension ref="A1:S414"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -15692,7 +15710,7 @@
       <c r="L2" t="s">
         <v>4959</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="3" t="s">
         <v>4960</v>
       </c>
       <c r="N2" t="s">
@@ -15748,34 +15766,34 @@
       <c r="L3" t="s">
         <v>4974</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="3" t="s">
+        <v>5085</v>
+      </c>
+      <c r="N3" t="s">
         <v>4975</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>4976</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>4977</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>4978</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>4979</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>4980</v>
-      </c>
-      <c r="S3" t="s">
-        <v>4981</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>4981</v>
+      </c>
+      <c r="B4" t="s">
         <v>4982</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4983</v>
       </c>
       <c r="C4" t="s">
         <v>4952</v>
@@ -15787,51 +15805,51 @@
         <v>4953</v>
       </c>
       <c r="F4" t="s">
+        <v>4983</v>
+      </c>
+      <c r="H4" t="s">
         <v>4984</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>4985</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>4986</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>4987</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>4988</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" s="3" t="s">
         <v>4989</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>4990</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>4991</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>4992</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>4993</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>4994</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>4995</v>
-      </c>
-      <c r="S4" t="s">
-        <v>4996</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>4996</v>
+      </c>
+      <c r="B5" t="s">
         <v>4997</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4998</v>
       </c>
       <c r="C5" t="s">
         <v>4952</v>
@@ -15860,7 +15878,7 @@
       <c r="L5" t="s">
         <v>4959</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="3" t="s">
         <v>4960</v>
       </c>
       <c r="N5" t="s">
@@ -15884,10 +15902,10 @@
     </row>
     <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>4998</v>
+      </c>
+      <c r="B6" t="s">
         <v>4999</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5000</v>
       </c>
       <c r="C6" t="s">
         <v>4952</v>
@@ -15916,34 +15934,34 @@
       <c r="L6" t="s">
         <v>4974</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="3" t="s">
+        <v>5085</v>
+      </c>
+      <c r="N6" t="s">
         <v>4975</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>4976</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>4977</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>4978</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>4979</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>4980</v>
-      </c>
-      <c r="S6" t="s">
-        <v>4981</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>5000</v>
+      </c>
+      <c r="B7" t="s">
         <v>5001</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5002</v>
       </c>
       <c r="C7" t="s">
         <v>4952</v>
@@ -15955,51 +15973,51 @@
         <v>4953</v>
       </c>
       <c r="F7" t="s">
+        <v>4983</v>
+      </c>
+      <c r="H7" t="s">
         <v>4984</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>4985</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>4986</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>4987</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>4988</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" s="3" t="s">
         <v>4989</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>4990</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>4991</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>4992</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>4993</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>4994</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>4995</v>
-      </c>
-      <c r="S7" t="s">
-        <v>4996</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>5002</v>
+      </c>
+      <c r="B8" t="s">
         <v>5003</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5004</v>
       </c>
       <c r="C8" t="s">
         <v>4952</v>
@@ -16028,7 +16046,7 @@
       <c r="L8" t="s">
         <v>4959</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M8" s="3" t="s">
         <v>4960</v>
       </c>
       <c r="N8" t="s">
@@ -16052,10 +16070,10 @@
     </row>
     <row r="9" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>5004</v>
+      </c>
+      <c r="B9" t="s">
         <v>5005</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5006</v>
       </c>
       <c r="C9" t="s">
         <v>4952</v>
@@ -16084,34 +16102,34 @@
       <c r="L9" t="s">
         <v>4974</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="3" t="s">
+        <v>5085</v>
+      </c>
+      <c r="N9" t="s">
         <v>4975</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>4976</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>4977</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>4978</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>4979</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>4980</v>
-      </c>
-      <c r="S9" t="s">
-        <v>4981</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>5006</v>
+      </c>
+      <c r="B10" t="s">
         <v>5007</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5008</v>
       </c>
       <c r="C10" t="s">
         <v>4952</v>
@@ -16123,61 +16141,61 @@
         <v>4953</v>
       </c>
       <c r="F10" t="s">
+        <v>4983</v>
+      </c>
+      <c r="H10" t="s">
         <v>4984</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>4985</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>4986</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>4987</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>4988</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" s="3" t="s">
         <v>4989</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>4990</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>4991</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>4992</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>4993</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>4994</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>4995</v>
-      </c>
-      <c r="S10" t="s">
-        <v>4996</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>5008</v>
+      </c>
+      <c r="B12" t="s">
         <v>5009</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>5010</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5011</v>
       </c>
       <c r="D12">
         <v>1702</v>
       </c>
       <c r="E12" t="s">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="F12" t="s">
         <v>4954</v>
@@ -16186,7 +16204,7 @@
         <v>4928</v>
       </c>
       <c r="I12" t="s">
-        <v>5013</v>
+        <v>5012</v>
       </c>
       <c r="J12" t="s">
         <v>4926</v>
@@ -16221,58 +16239,58 @@
     </row>
     <row r="13" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>5013</v>
+      </c>
+      <c r="B13" t="s">
         <v>5014</v>
       </c>
-      <c r="B13" t="s">
-        <v>5015</v>
-      </c>
       <c r="C13" t="s">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="D13">
         <v>1702</v>
       </c>
       <c r="E13" t="s">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="F13" t="s">
         <v>4969</v>
       </c>
       <c r="H13" t="s">
+        <v>5015</v>
+      </c>
+      <c r="I13" t="s">
         <v>5016</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>5017</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>5018</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>5019</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>5020</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>5021</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>5022</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>5023</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" t="s">
         <v>5024</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>5025</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>5026</v>
-      </c>
-      <c r="S13" t="s">
-        <v>5027</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -19843,19 +19861,19 @@
     <row r="76" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>5027</v>
+      </c>
+      <c r="B77" t="s">
         <v>5028</v>
       </c>
-      <c r="B77" t="s">
-        <v>5029</v>
-      </c>
       <c r="C77" t="s">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="D77">
         <v>1703</v>
       </c>
       <c r="E77" t="s">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="F77" t="s">
         <v>4954</v>
@@ -19864,7 +19882,7 @@
         <v>4118</v>
       </c>
       <c r="I77" t="s">
-        <v>5030</v>
+        <v>5029</v>
       </c>
       <c r="J77" t="s">
         <v>4116</v>
@@ -19899,58 +19917,58 @@
     </row>
     <row r="78" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>5030</v>
+      </c>
+      <c r="B78" t="s">
         <v>5031</v>
       </c>
-      <c r="B78" t="s">
-        <v>5032</v>
-      </c>
       <c r="C78" t="s">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="D78">
         <v>1703</v>
       </c>
       <c r="E78" t="s">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="F78" t="s">
         <v>4969</v>
       </c>
       <c r="H78" t="s">
+        <v>5032</v>
+      </c>
+      <c r="I78" t="s">
         <v>5033</v>
       </c>
-      <c r="I78" t="s">
+      <c r="J78" t="s">
         <v>5034</v>
       </c>
-      <c r="J78" t="s">
+      <c r="K78" t="s">
         <v>5035</v>
       </c>
-      <c r="K78" t="s">
+      <c r="L78" t="s">
         <v>5036</v>
       </c>
-      <c r="L78" t="s">
+      <c r="M78" t="s">
         <v>5037</v>
       </c>
-      <c r="M78" t="s">
+      <c r="N78" t="s">
         <v>5038</v>
       </c>
-      <c r="N78" t="s">
+      <c r="O78" t="s">
         <v>5039</v>
       </c>
-      <c r="O78" t="s">
+      <c r="P78" t="s">
         <v>5040</v>
       </c>
-      <c r="P78" t="s">
+      <c r="Q78" t="s">
         <v>5041</v>
       </c>
-      <c r="Q78" t="s">
+      <c r="R78" t="s">
         <v>5042</v>
       </c>
-      <c r="R78" t="s">
+      <c r="S78" t="s">
         <v>5043</v>
-      </c>
-      <c r="S78" t="s">
-        <v>5044</v>
       </c>
     </row>
     <row r="79" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -26214,19 +26232,19 @@
     <row r="187" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="188" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
+        <v>5044</v>
+      </c>
+      <c r="B188" t="s">
         <v>5045</v>
       </c>
-      <c r="B188" t="s">
-        <v>5046</v>
-      </c>
       <c r="C188" t="s">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="D188">
         <v>1704</v>
       </c>
       <c r="E188" t="s">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="F188" t="s">
         <v>4954</v>
@@ -26235,7 +26253,7 @@
         <v>2717</v>
       </c>
       <c r="I188" t="s">
-        <v>5047</v>
+        <v>5046</v>
       </c>
       <c r="J188" t="s">
         <v>2715</v>
@@ -26270,75 +26288,75 @@
     </row>
     <row r="189" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
+        <v>5047</v>
+      </c>
+      <c r="B189" t="s">
         <v>5048</v>
       </c>
-      <c r="B189" t="s">
-        <v>5049</v>
-      </c>
       <c r="C189" t="s">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="D189">
         <v>1704</v>
       </c>
       <c r="E189" t="s">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="F189" t="s">
         <v>4969</v>
       </c>
       <c r="H189" t="s">
+        <v>5049</v>
+      </c>
+      <c r="I189" t="s">
         <v>5050</v>
       </c>
-      <c r="I189" t="s">
+      <c r="J189" t="s">
         <v>5051</v>
       </c>
-      <c r="J189" t="s">
+      <c r="K189" t="s">
         <v>5052</v>
       </c>
-      <c r="K189" t="s">
+      <c r="L189" t="s">
         <v>5053</v>
       </c>
-      <c r="L189" t="s">
+      <c r="M189" t="s">
         <v>5054</v>
       </c>
-      <c r="M189" t="s">
+      <c r="N189" t="s">
         <v>5055</v>
       </c>
-      <c r="N189" t="s">
+      <c r="O189" t="s">
         <v>5056</v>
       </c>
-      <c r="O189" t="s">
+      <c r="P189" t="s">
         <v>5057</v>
       </c>
-      <c r="P189" t="s">
+      <c r="Q189" t="s">
         <v>5058</v>
       </c>
-      <c r="Q189" t="s">
+      <c r="R189" t="s">
         <v>5059</v>
       </c>
-      <c r="R189" t="s">
+      <c r="S189" t="s">
         <v>5060</v>
-      </c>
-      <c r="S189" t="s">
-        <v>5061</v>
       </c>
     </row>
     <row r="190" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
+        <v>5061</v>
+      </c>
+      <c r="B190" t="s">
         <v>5062</v>
       </c>
-      <c r="B190" t="s">
-        <v>5063</v>
-      </c>
       <c r="C190" t="s">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="D190">
         <v>1706</v>
       </c>
       <c r="E190" t="s">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="F190" t="s">
         <v>4954</v>
@@ -26347,7 +26365,7 @@
         <v>2717</v>
       </c>
       <c r="I190" t="s">
-        <v>5047</v>
+        <v>5046</v>
       </c>
       <c r="J190" t="s">
         <v>2715</v>
@@ -26382,75 +26400,75 @@
     </row>
     <row r="191" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
+        <v>5063</v>
+      </c>
+      <c r="B191" t="s">
         <v>5064</v>
       </c>
-      <c r="B191" t="s">
-        <v>5065</v>
-      </c>
       <c r="C191" t="s">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="D191">
         <v>1706</v>
       </c>
       <c r="E191" t="s">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="F191" t="s">
         <v>4969</v>
       </c>
       <c r="H191" t="s">
+        <v>5049</v>
+      </c>
+      <c r="I191" t="s">
         <v>5050</v>
       </c>
-      <c r="I191" t="s">
+      <c r="J191" t="s">
         <v>5051</v>
       </c>
-      <c r="J191" t="s">
+      <c r="K191" t="s">
         <v>5052</v>
       </c>
-      <c r="K191" t="s">
+      <c r="L191" t="s">
         <v>5053</v>
       </c>
-      <c r="L191" t="s">
+      <c r="M191" t="s">
         <v>5054</v>
       </c>
-      <c r="M191" t="s">
+      <c r="N191" t="s">
         <v>5055</v>
       </c>
-      <c r="N191" t="s">
+      <c r="O191" t="s">
         <v>5056</v>
       </c>
-      <c r="O191" t="s">
+      <c r="P191" t="s">
         <v>5057</v>
       </c>
-      <c r="P191" t="s">
+      <c r="Q191" t="s">
         <v>5058</v>
       </c>
-      <c r="Q191" t="s">
+      <c r="R191" t="s">
         <v>5059</v>
       </c>
-      <c r="R191" t="s">
+      <c r="S191" t="s">
         <v>5060</v>
-      </c>
-      <c r="S191" t="s">
-        <v>5061</v>
       </c>
     </row>
     <row r="192" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
+        <v>5065</v>
+      </c>
+      <c r="B192" t="s">
         <v>5066</v>
       </c>
-      <c r="B192" t="s">
-        <v>5067</v>
-      </c>
       <c r="C192" t="s">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="D192">
         <v>1707</v>
       </c>
       <c r="E192" t="s">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="F192" t="s">
         <v>4954</v>
@@ -26459,7 +26477,7 @@
         <v>2717</v>
       </c>
       <c r="I192" t="s">
-        <v>5047</v>
+        <v>5046</v>
       </c>
       <c r="J192" t="s">
         <v>2715</v>
@@ -26494,58 +26512,58 @@
     </row>
     <row r="193" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
+        <v>5067</v>
+      </c>
+      <c r="B193" t="s">
         <v>5068</v>
       </c>
-      <c r="B193" t="s">
-        <v>5069</v>
-      </c>
       <c r="C193" t="s">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="D193">
         <v>1707</v>
       </c>
       <c r="E193" t="s">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="F193" t="s">
         <v>4969</v>
       </c>
       <c r="H193" t="s">
+        <v>5049</v>
+      </c>
+      <c r="I193" t="s">
         <v>5050</v>
       </c>
-      <c r="I193" t="s">
+      <c r="J193" t="s">
         <v>5051</v>
       </c>
-      <c r="J193" t="s">
+      <c r="K193" t="s">
         <v>5052</v>
       </c>
-      <c r="K193" t="s">
+      <c r="L193" t="s">
         <v>5053</v>
       </c>
-      <c r="L193" t="s">
+      <c r="M193" t="s">
         <v>5054</v>
       </c>
-      <c r="M193" t="s">
+      <c r="N193" t="s">
         <v>5055</v>
       </c>
-      <c r="N193" t="s">
+      <c r="O193" t="s">
         <v>5056</v>
       </c>
-      <c r="O193" t="s">
+      <c r="P193" t="s">
         <v>5057</v>
       </c>
-      <c r="P193" t="s">
+      <c r="Q193" t="s">
         <v>5058</v>
       </c>
-      <c r="Q193" t="s">
+      <c r="R193" t="s">
         <v>5059</v>
       </c>
-      <c r="R193" t="s">
+      <c r="S193" t="s">
         <v>5060</v>
-      </c>
-      <c r="S193" t="s">
-        <v>5061</v>
       </c>
     </row>
     <row r="194" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -33202,19 +33220,19 @@
     <row r="313" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="314" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>5085</v>
+        <v>5084</v>
       </c>
       <c r="B314" t="s">
-        <v>5084</v>
+        <v>5083</v>
       </c>
       <c r="C314" t="s">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="D314">
         <v>1705</v>
       </c>
       <c r="E314" t="s">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="F314" t="s">
         <v>4954</v>
@@ -33258,58 +33276,58 @@
     </row>
     <row r="315" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>5083</v>
+        <v>5082</v>
       </c>
       <c r="B315" t="s">
-        <v>5082</v>
+        <v>5081</v>
       </c>
       <c r="C315" t="s">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="D315">
         <v>1705</v>
       </c>
       <c r="E315" t="s">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="F315" t="s">
         <v>4969</v>
       </c>
       <c r="H315" t="s">
-        <v>5081</v>
+        <v>5080</v>
       </c>
       <c r="I315" t="s">
-        <v>5080</v>
+        <v>5079</v>
       </c>
       <c r="J315" t="s">
-        <v>5079</v>
+        <v>5078</v>
       </c>
       <c r="K315" t="s">
-        <v>5078</v>
+        <v>5077</v>
       </c>
       <c r="L315" t="s">
-        <v>5077</v>
+        <v>5076</v>
       </c>
       <c r="M315" t="s">
-        <v>5076</v>
+        <v>5075</v>
       </c>
       <c r="N315" t="s">
-        <v>5075</v>
+        <v>5074</v>
       </c>
       <c r="O315" t="s">
-        <v>5074</v>
+        <v>5073</v>
       </c>
       <c r="P315" t="s">
-        <v>5073</v>
+        <v>5072</v>
       </c>
       <c r="Q315" t="s">
-        <v>5072</v>
+        <v>5071</v>
       </c>
       <c r="R315" t="s">
-        <v>5071</v>
+        <v>5070</v>
       </c>
       <c r="S315" t="s">
-        <v>5070</v>
+        <v>5069</v>
       </c>
     </row>
     <row r="316" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>